<commit_message>
feat: add the initial supporting material suggested by Thomas feat: properly render links in education items for the exercise widget
</commit_message>
<xml_diff>
--- a/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
+++ b/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carbon\development\cs-aware-next-cs-connect\cs-faker-data-provider\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E975099A-1612-48AD-9800-8546360BC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Data 1"/>
-    <sheet r:id="rId2" sheetId="2" name="data as rows"/>
+    <sheet name="Data 1" sheetId="1" r:id="rId1"/>
+    <sheet name="data as rows" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Case</t>
   </si>
@@ -119,15 +125,23 @@
     <t>Supporting material</t>
   </si>
   <si>
-    <t>To be decided</t>
+    <t>https://www.youtube.com/watch?v=kbMPG6eYjhc</t>
+  </si>
+  <si>
+    <t>https://www.pdq.com/blog/deploying-software-best-practices/</t>
+  </si>
+  <si>
+    <t>https://www.parkplacetechnologies.com/blog/enterprise-server-patch-management-best-practices/</t>
+  </si>
+  <si>
+    <t>https://www.cisa.gov/secure-our-world/update-software</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +168,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="CIDFont+F1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -164,7 +199,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -178,16 +213,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -199,59 +234,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -262,10 +302,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -303,71 +343,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,7 +435,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -418,11 +458,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -431,13 +471,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -447,7 +487,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -456,7 +496,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -465,7 +505,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -473,10 +513,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -541,231 +581,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="651.75" customFormat="1" s="7">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="409.6" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="12" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="U1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T1" r:id="rId1" xr:uid="{E3D88D9E-E4A1-4158-98F2-18DF003469A6}"/>
+    <hyperlink ref="U1" r:id="rId2" xr:uid="{F7F3CBD3-C4F9-4829-9998-63C1291E1B21}"/>
+    <hyperlink ref="V1" r:id="rId3" xr:uid="{4863D1AB-718C-4A59-B237-3C02F2815553}"/>
+    <hyperlink ref="S1" r:id="rId4" xr:uid="{DF65838B-2EB5-4D6C-86ED-715DC1BC8C1B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:1" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:1" ht="17.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:1" ht="17.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:1" ht="17.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:1" ht="17.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:1" ht="17.25" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:1" ht="17.25" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:1" ht="17.25" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:1" ht="17.25" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:1" ht="17.25" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="12" spans="1:1" ht="17.25" customHeight="1"/>
+    <row r="13" spans="1:1" ht="17.25" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:1" ht="17.25" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:1" ht="17.25" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:1" ht="17.25" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:1" ht="17.25" customHeight="1">
       <c r="A17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:1" ht="17.25" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:1" ht="17.25" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:1" ht="17.25" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:1" ht="17.25" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:1" ht="17.25" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:1" ht="17.25" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
-      <c r="A24" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="24" spans="1:1" ht="17.25" customHeight="1"/>
+    <row r="25" spans="1:1" ht="17.25" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="1:1" ht="75">
+      <c r="A26" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="75">
+      <c r="A27" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="90">
+      <c r="A28" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="135">
+      <c r="A29" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A26" r:id="rId1" xr:uid="{BBD4BC18-127B-4AEF-936A-68C1FED01156}"/>
+    <hyperlink ref="A27" r:id="rId2" xr:uid="{AB8B9FBF-B55B-4725-9F91-9B8BA2F8AAB6}"/>
+    <hyperlink ref="A28" r:id="rId3" xr:uid="{43D86ED1-B928-412D-923B-90B3850DC415}"/>
+    <hyperlink ref="A29" r:id="rId4" xr:uid="{125C7AD2-0752-499D-A031-D259AB12A010}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: adds italian supporting material for foggia exercise
</commit_message>
<xml_diff>
--- a/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
+++ b/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carbon\development\cs-aware-next-cs-connect\cs-faker-data-provider\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E975099A-1612-48AD-9800-8546360BC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD2C58-8EB9-46CB-B447-EE14BC8BC19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Case</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>https://www.cisa.gov/secure-our-world/update-software</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/it-it/topics/patch-management</t>
+  </si>
+  <si>
+    <t>https://cpl.thalesgroup.com/it/software-monetization/what-is-patch-management</t>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -279,6 +285,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -585,10 +592,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,7 +603,7 @@
     <col min="1" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" ht="409.6" customHeight="1">
+    <row r="1" spans="1:24" s="6" customFormat="1" ht="409.6" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -658,6 +665,12 @@
       </c>
       <c r="V1" s="13" t="s">
         <v>25</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -666,6 +679,8 @@
     <hyperlink ref="U1" r:id="rId2" xr:uid="{F7F3CBD3-C4F9-4829-9998-63C1291E1B21}"/>
     <hyperlink ref="V1" r:id="rId3" xr:uid="{4863D1AB-718C-4A59-B237-3C02F2815553}"/>
     <hyperlink ref="S1" r:id="rId4" xr:uid="{DF65838B-2EB5-4D6C-86ED-715DC1BC8C1B}"/>
+    <hyperlink ref="W1" r:id="rId5" xr:uid="{2610682C-6C09-4361-99E3-980DB0C12A41}"/>
+    <hyperlink ref="X1" r:id="rId6" xr:uid="{D915B319-194D-4DB6-AF54-2BA327DD6678}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -676,10 +691,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,14 +837,26 @@
         <v>25</v>
       </c>
     </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A26" r:id="rId1" xr:uid="{BBD4BC18-127B-4AEF-936A-68C1FED01156}"/>
     <hyperlink ref="A27" r:id="rId2" xr:uid="{AB8B9FBF-B55B-4725-9F91-9B8BA2F8AAB6}"/>
     <hyperlink ref="A28" r:id="rId3" xr:uid="{43D86ED1-B928-412D-923B-90B3850DC415}"/>
     <hyperlink ref="A29" r:id="rId4" xr:uid="{125C7AD2-0752-499D-A031-D259AB12A010}"/>
+    <hyperlink ref="A30" r:id="rId5" xr:uid="{80E7B7D4-E7FF-410E-81BC-DB94C192ACCA}"/>
+    <hyperlink ref="A31" r:id="rId6" xr:uid="{8C08F8EE-1C14-48EB-8895-3E46A45E2040}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: localized foggia exercise data in italian, added descriptions for supporting data
</commit_message>
<xml_diff>
--- a/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
+++ b/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carbon\development\cs-aware-next-cs-connect\cs-faker-data-provider\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD2C58-8EB9-46CB-B447-EE14BC8BC19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3FF13-9724-47E8-9CBC-596E484A5A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6270" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Case</t>
   </si>
@@ -141,6 +141,57 @@
   </si>
   <si>
     <t>https://cpl.thalesgroup.com/it/software-monetization/what-is-patch-management</t>
+  </si>
+  <si>
+    <t>Informazioni di alto livello sugli aggiornamenti software:</t>
+  </si>
+  <si>
+    <t>Manutenzione del software:</t>
+  </si>
+  <si>
+    <t>Migliori pratiche di aggiornamento software da un contesto organizzativo (entrambi sono blog di società commerciali, il progetto non è affiliato)</t>
+  </si>
+  <si>
+    <t>Cos'è la gestione delle patch? (risorse in italiano)</t>
+  </si>
+  <si>
+    <t>All'interno della struttura X, il reparto contabilità utilizza un'applicazione software e un database legacy che funzionano solo su un sistema operativo (SO) obsoleto. In esecuzione su una macchina virtuale (VM), questo sistema operativo è stato interrotto (non è più supportato dal produttore) e presenta vulnerabilità di sicurezza note. All'interno del reparto contabilità, tutti i computer hanno accesso a Internet, inclusa la VM che ospita il sistema operativo legacy.</t>
+  </si>
+  <si>
+    <t>Utilizzando tecniche di propagazione che sfruttano le vulnerabilità nei protocolli di rete, il malware si diffonde nella rete colpendo diversi computer desktop e server collegati.</t>
+  </si>
+  <si>
+    <t>I sistemi informativi dell'organizzazione mostrano una risposta lenta e un'elevata latenza.</t>
+  </si>
+  <si>
+    <t>A poco a poco, gli utenti non possono accedere ai propri computer e accedere ai sistemi informativi.</t>
+  </si>
+  <si>
+    <t>Man mano che l’attacco si diffonde, a tutto il personale viene ordinato di smettere di utilizzare i sistemi digitalizzati e l’infrastruttura IT e di passare alle operazioni cartacee.</t>
+  </si>
+  <si>
+    <t>In risposta all'attacco, il reparto IT spegne l'intera infrastruttura informatica e procede con un'installazione pulita dei computer, ricorrendo a sistemi di backup per recuperare parzialmente i dati ospedalieri.</t>
+  </si>
+  <si>
+    <t>Il tempo di ripristino previsto è stimato in 2 o 3 giorni lavorativi, a seconda del numero di asset interessati e dello sforzo richiesto per reinstallare l'infrastruttura IT.</t>
+  </si>
+  <si>
+    <t>2. Gestione del rischio: quali sarebbero le politiche, le conoscenze, le informazioni o le azioni necessarie di cui questa organizzazione e le persone menzionate hanno bisogno per evitare che il problema si verifichi?</t>
+  </si>
+  <si>
+    <t>3. Potrebbe succedere nella tua organizzazione? Perché/perché no?</t>
+  </si>
+  <si>
+    <t>Il malware crea botnet e provoca fenomeni a valanga (ad es. congestione della rete locale e dei server, blocco degli account utente) che rendono l'infrastruttura IT non operativa.</t>
+  </si>
+  <si>
+    <t>Il dipendente utilizza quotidianamente questa VM per svolgere il suo lavoro. Occasionalmente utilizza la VM anche per navigare in Internet e accidentalmente scarica ed esegue un'applicazione infettata da un malware (ad esempio il malware Conficker), attivandolo.</t>
+  </si>
+  <si>
+    <t>4. Quale sarebbe l'impatto potenziale se ciò accadesse alla tua organizzazione?</t>
+  </si>
+  <si>
+    <t>1. Gestione degli incidenti: quali sono i passaggi specifici necessari per risolvere il problema? Includere i ruoli del dipartimento IT, IT e altri dirigenti, personale. Puoi fare un elenco di passaggi (paralleli) da eseguire?</t>
   </si>
 </sst>
 </file>
@@ -196,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -244,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,6 +343,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -592,18 +652,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" ht="409.6" customHeight="1">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="409.6" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -611,76 +673,92 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="N1" s="9" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="R1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="W1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="Z1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T1" r:id="rId1" xr:uid="{E3D88D9E-E4A1-4158-98F2-18DF003469A6}"/>
-    <hyperlink ref="U1" r:id="rId2" xr:uid="{F7F3CBD3-C4F9-4829-9998-63C1291E1B21}"/>
-    <hyperlink ref="V1" r:id="rId3" xr:uid="{4863D1AB-718C-4A59-B237-3C02F2815553}"/>
-    <hyperlink ref="S1" r:id="rId4" xr:uid="{DF65838B-2EB5-4D6C-86ED-715DC1BC8C1B}"/>
-    <hyperlink ref="W1" r:id="rId5" xr:uid="{2610682C-6C09-4361-99E3-980DB0C12A41}"/>
-    <hyperlink ref="X1" r:id="rId6" xr:uid="{D915B319-194D-4DB6-AF54-2BA327DD6678}"/>
+    <hyperlink ref="V1" r:id="rId1" xr:uid="{E3D88D9E-E4A1-4158-98F2-18DF003469A6}"/>
+    <hyperlink ref="X1" r:id="rId2" xr:uid="{F7F3CBD3-C4F9-4829-9998-63C1291E1B21}"/>
+    <hyperlink ref="Y1" r:id="rId3" xr:uid="{4863D1AB-718C-4A59-B237-3C02F2815553}"/>
+    <hyperlink ref="T1" r:id="rId4" xr:uid="{DF65838B-2EB5-4D6C-86ED-715DC1BC8C1B}"/>
+    <hyperlink ref="AA1" r:id="rId5" xr:uid="{2610682C-6C09-4361-99E3-980DB0C12A41}"/>
+    <hyperlink ref="AB1" r:id="rId6" xr:uid="{D915B319-194D-4DB6-AF54-2BA327DD6678}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -693,7 +771,7 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: cleaned Foggia exercise data
</commit_message>
<xml_diff>
--- a/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
+++ b/cs-faker-data-provider/data/foggia-exercise-ccc12c9a-8b99-48d8-b97e-5e1eec042b4f.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carbon\development\cs-aware-next-cs-connect\cs-faker-data-provider\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3FF13-9724-47E8-9CBC-596E484A5A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data 1" sheetId="1" r:id="rId1"/>
-    <sheet name="data as rows" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="Data 1"/>
+    <sheet r:id="rId2" sheetId="2" name="data as rows"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Case</t>
   </si>
@@ -122,83 +116,84 @@
     <t>Educational material</t>
   </si>
   <si>
+    <t>https://www.cisa.gov/secure-our-world/update-software</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kbMPG6eYjhc</t>
+  </si>
+  <si>
+    <t>https://www.pdq.com/blog/deploying-software-best-practices/</t>
+  </si>
+  <si>
+    <t>https://www.parkplacetechnologies.com/blog/enterprise-server-patch-management-best-practices/</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/it-it/topics/patch-management</t>
+  </si>
+  <si>
+    <t>https://cpl.thalesgroup.com/it/software-monetization/what-is-patch-management</t>
+  </si>
+  <si>
+    <t>All'interno della struttura X, il reparto contabilità utilizza un'applicazione software e un database legacy che funzionano solo su un sistema operativo (SO) obsoleto. In esecuzione su una macchina virtuale (VM), questo sistema operativo è stato interrotto (non è più supportato dal produttore) e presenta vulnerabilità di sicurezza note. All'interno del reparto contabilità, tutti i computer hanno accesso a Internet, inclusa la VM che ospita il sistema operativo legacy.</t>
+  </si>
+  <si>
+    <t>Il dipendente utilizza quotidianamente questa VM per svolgere il suo lavoro. Occasionalmente utilizza la VM anche per navigare in Internet e accidentalmente scarica ed esegue un'applicazione infettata da un malware (ad esempio il malware Conficker), attivandolo.</t>
+  </si>
+  <si>
+    <t>Utilizzando tecniche di propagazione che sfruttano le vulnerabilità nei protocolli di rete, il malware si diffonde nella rete colpendo diversi computer desktop e server collegati.</t>
+  </si>
+  <si>
+    <t>Il malware crea botnet e provoca fenomeni a valanga (ad es. congestione della rete locale e dei server, blocco degli account utente) che rendono l'infrastruttura IT non operativa.</t>
+  </si>
+  <si>
+    <t>I sistemi informativi dell'organizzazione mostrano una risposta lenta e un'elevata latenza.</t>
+  </si>
+  <si>
+    <t>A poco a poco, gli utenti non possono accedere ai propri computer e accedere ai sistemi informativi.</t>
+  </si>
+  <si>
+    <t>Man mano che l’attacco si diffonde, a tutto il personale viene ordinato di smettere di utilizzare i sistemi digitalizzati e l’infrastruttura IT e di passare alle operazioni cartacee.</t>
+  </si>
+  <si>
+    <t>In risposta all'attacco, il reparto IT spegne l'intera infrastruttura informatica e procede con un'installazione pulita dei computer, ricorrendo a sistemi di backup per recuperare parzialmente i dati ospedalieri.</t>
+  </si>
+  <si>
+    <t>Il tempo di ripristino previsto è stimato in 2 o 3 giorni lavorativi, a seconda del numero di asset interessati e dello sforzo richiesto per reinstallare l'infrastruttura IT.</t>
+  </si>
+  <si>
+    <t>1. Gestione degli incidenti: quali sono i passaggi specifici necessari per risolvere il problema? Includere i ruoli del dipartimento IT, IT e altri dirigenti, personale. Puoi fare un elenco di passaggi (paralleli) da eseguire?</t>
+  </si>
+  <si>
+    <t>2. Gestione del rischio: quali sarebbero le politiche, le conoscenze, le informazioni o le azioni necessarie di cui questa organizzazione e le persone menzionate hanno bisogno per evitare che il problema si verifichi?</t>
+  </si>
+  <si>
+    <t>3. Potrebbe succedere nella tua organizzazione? Perché/perché no?</t>
+  </si>
+  <si>
+    <t>4. Quale sarebbe l'impatto potenziale se ciò accadesse alla tua organizzazione?</t>
+  </si>
+  <si>
     <t>Supporting material</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=kbMPG6eYjhc</t>
-  </si>
-  <si>
-    <t>https://www.pdq.com/blog/deploying-software-best-practices/</t>
-  </si>
-  <si>
-    <t>https://www.parkplacetechnologies.com/blog/enterprise-server-patch-management-best-practices/</t>
-  </si>
-  <si>
-    <t>https://www.cisa.gov/secure-our-world/update-software</t>
-  </si>
-  <si>
-    <t>https://www.ibm.com/it-it/topics/patch-management</t>
-  </si>
-  <si>
-    <t>https://cpl.thalesgroup.com/it/software-monetization/what-is-patch-management</t>
-  </si>
-  <si>
-    <t>Informazioni di alto livello sugli aggiornamenti software:</t>
-  </si>
-  <si>
-    <t>Manutenzione del software:</t>
+    <t>Informazioni di alto livello sugli aggiornamenti software: https://www.cisa.gov/secure-our-world/update-software</t>
+  </si>
+  <si>
+    <t>Manutenzione del software: https://www.youtube.com/watch?v=kbMPG6eYjhc</t>
   </si>
   <si>
     <t>Migliori pratiche di aggiornamento software da un contesto organizzativo (entrambi sono blog di società commerciali, il progetto non è affiliato)</t>
   </si>
   <si>
     <t>Cos'è la gestione delle patch? (risorse in italiano)</t>
-  </si>
-  <si>
-    <t>All'interno della struttura X, il reparto contabilità utilizza un'applicazione software e un database legacy che funzionano solo su un sistema operativo (SO) obsoleto. In esecuzione su una macchina virtuale (VM), questo sistema operativo è stato interrotto (non è più supportato dal produttore) e presenta vulnerabilità di sicurezza note. All'interno del reparto contabilità, tutti i computer hanno accesso a Internet, inclusa la VM che ospita il sistema operativo legacy.</t>
-  </si>
-  <si>
-    <t>Utilizzando tecniche di propagazione che sfruttano le vulnerabilità nei protocolli di rete, il malware si diffonde nella rete colpendo diversi computer desktop e server collegati.</t>
-  </si>
-  <si>
-    <t>I sistemi informativi dell'organizzazione mostrano una risposta lenta e un'elevata latenza.</t>
-  </si>
-  <si>
-    <t>A poco a poco, gli utenti non possono accedere ai propri computer e accedere ai sistemi informativi.</t>
-  </si>
-  <si>
-    <t>Man mano che l’attacco si diffonde, a tutto il personale viene ordinato di smettere di utilizzare i sistemi digitalizzati e l’infrastruttura IT e di passare alle operazioni cartacee.</t>
-  </si>
-  <si>
-    <t>In risposta all'attacco, il reparto IT spegne l'intera infrastruttura informatica e procede con un'installazione pulita dei computer, ricorrendo a sistemi di backup per recuperare parzialmente i dati ospedalieri.</t>
-  </si>
-  <si>
-    <t>Il tempo di ripristino previsto è stimato in 2 o 3 giorni lavorativi, a seconda del numero di asset interessati e dello sforzo richiesto per reinstallare l'infrastruttura IT.</t>
-  </si>
-  <si>
-    <t>2. Gestione del rischio: quali sarebbero le politiche, le conoscenze, le informazioni o le azioni necessarie di cui questa organizzazione e le persone menzionate hanno bisogno per evitare che il problema si verifichi?</t>
-  </si>
-  <si>
-    <t>3. Potrebbe succedere nella tua organizzazione? Perché/perché no?</t>
-  </si>
-  <si>
-    <t>Il malware crea botnet e provoca fenomeni a valanga (ad es. congestione della rete locale e dei server, blocco degli account utente) che rendono l'infrastruttura IT non operativa.</t>
-  </si>
-  <si>
-    <t>Il dipendente utilizza quotidianamente questa VM per svolgere il suo lavoro. Occasionalmente utilizza la VM anche per navigare in Internet e accidentalmente scarica ed esegue un'applicazione infettata da un malware (ad esempio il malware Conficker), attivandolo.</t>
-  </si>
-  <si>
-    <t>4. Quale sarebbe l'impatto potenziale se ciò accadesse alla tua organizzazione?</t>
-  </si>
-  <si>
-    <t>1. Gestione degli incidenti: quali sono i passaggi specifici necessari per risolvere il problema? Includere i ruoli del dipartimento IT, IT e altri dirigenti, personale. Puoi fare un elenco di passaggi (paralleli) da eseguire?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,25 +221,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="CIDFont+F1"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -256,13 +237,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,16 +256,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -297,68 +277,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -369,10 +349,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -410,71 +390,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,7 +482,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -525,11 +505,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -538,13 +518,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -554,7 +534,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -563,7 +543,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -572,7 +552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -580,10 +560,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -648,293 +628,293 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="409.6" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="693" customFormat="1" s="6">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="I1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="U1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="12" t="s">
+      <c r="Y1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="14" t="s">
+      <c r="Z1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="14" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V1" r:id="rId1" xr:uid="{E3D88D9E-E4A1-4158-98F2-18DF003469A6}"/>
-    <hyperlink ref="X1" r:id="rId2" xr:uid="{F7F3CBD3-C4F9-4829-9998-63C1291E1B21}"/>
-    <hyperlink ref="Y1" r:id="rId3" xr:uid="{4863D1AB-718C-4A59-B237-3C02F2815553}"/>
-    <hyperlink ref="T1" r:id="rId4" xr:uid="{DF65838B-2EB5-4D6C-86ED-715DC1BC8C1B}"/>
-    <hyperlink ref="AA1" r:id="rId5" xr:uid="{2610682C-6C09-4361-99E3-980DB0C12A41}"/>
-    <hyperlink ref="AB1" r:id="rId6" xr:uid="{D915B319-194D-4DB6-AF54-2BA327DD6678}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17.25" customHeight="1"/>
-    <row r="13" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="17.25" customHeight="1"/>
-    <row r="25" spans="1:1" ht="17.25" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="75">
-      <c r="A26" s="12" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="6">
+      <c r="A26" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="6">
+      <c r="A27" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="6">
+      <c r="A28" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="6">
+      <c r="A29" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="75">
-      <c r="A27" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="90">
-      <c r="A28" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="135">
-      <c r="A29" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="14" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1" xr:uid="{BBD4BC18-127B-4AEF-936A-68C1FED01156}"/>
-    <hyperlink ref="A27" r:id="rId2" xr:uid="{AB8B9FBF-B55B-4725-9F91-9B8BA2F8AAB6}"/>
-    <hyperlink ref="A28" r:id="rId3" xr:uid="{43D86ED1-B928-412D-923B-90B3850DC415}"/>
-    <hyperlink ref="A29" r:id="rId4" xr:uid="{125C7AD2-0752-499D-A031-D259AB12A010}"/>
-    <hyperlink ref="A30" r:id="rId5" xr:uid="{80E7B7D4-E7FF-410E-81BC-DB94C192ACCA}"/>
-    <hyperlink ref="A31" r:id="rId6" xr:uid="{8C08F8EE-1C14-48EB-8895-3E46A45E2040}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>